<commit_message>
update params and doc
</commit_message>
<xml_diff>
--- a/billboard/ParamList.xlsx
+++ b/billboard/ParamList.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sustc-my.sharepoint.com/personal/12111524_mail_sustech_edu_cn/Documents/DeepScience/202407 iSURE/GitHub/Characterization-and-Modeling-of-GaN-HEMT/billboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C1754BF-08A8-AC40-B024-D6492DE63801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{1C1754BF-08A8-AC40-B024-D6492DE63801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1197CC8A-5878-4848-B38C-4883879ECDDF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{88C781BB-EB5C-664D-9596-BAFDE7D24BFC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{88C781BB-EB5C-664D-9596-BAFDE7D24BFC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Significant" sheetId="2" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="199">
   <si>
     <t>Idsmod</t>
   </si>
@@ -476,13 +477,169 @@
   </si>
   <si>
     <t>1·</t>
+  </si>
+  <si>
+    <t>最大gm处，id电流的值</t>
+  </si>
+  <si>
+    <t>最大gm处，Vg的值</t>
+  </si>
+  <si>
+    <t>delta gate voltage at peak gm</t>
+  </si>
+  <si>
+    <t>参数</t>
+  </si>
+  <si>
+    <t>saturation parameter alpha r</t>
+  </si>
+  <si>
+    <t>saturation parameter alpha</t>
+  </si>
+  <si>
+    <t>channel length modulation parameter</t>
+  </si>
+  <si>
+    <t>ICC</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>TUN</t>
+  </si>
+  <si>
+    <t>id的大小</t>
+  </si>
+  <si>
+    <t>对DC的影响</t>
+  </si>
+  <si>
+    <t>对S参数的影响</t>
+  </si>
+  <si>
+    <t>开启区域的斜率和曲线离散程度</t>
+  </si>
+  <si>
+    <t>定义与提取</t>
+  </si>
+  <si>
+    <t>开启区域到饱和区域的过渡是否尖锐</t>
+  </si>
+  <si>
+    <t>饱和区域斜率</t>
+  </si>
+  <si>
+    <t>0-bias D-S capacitance</t>
+  </si>
+  <si>
+    <t>G-S pinch off capacitance</t>
+  </si>
+  <si>
+    <t>G-S capacitance param</t>
+  </si>
+  <si>
+    <t>G-D pinch off capacitance</t>
+  </si>
+  <si>
+    <t>G-D capacitance param</t>
+  </si>
+  <si>
+    <t>External G-D capacitance</t>
+  </si>
+  <si>
+    <t>Polynomial coeff for channel current</t>
+  </si>
+  <si>
+    <t>Polynomial coeff for channel current，峰值gm处的gm/id</t>
+  </si>
+  <si>
+    <t>Polynomial coeff for capacitance</t>
+  </si>
+  <si>
+    <t>Gate fwd saturation current</t>
+  </si>
+  <si>
+    <t>Gate resistance</t>
+  </si>
+  <si>
+    <t>Drain resistance</t>
+  </si>
+  <si>
+    <t>Source resistance</t>
+  </si>
+  <si>
+    <t>Input resistance</t>
+  </si>
+  <si>
+    <t>S11和S22幅值，越大越小；S21和S12离散程度和相位差，越大越小</t>
+  </si>
+  <si>
+    <t>S11幅值，越大越小；S21和S12的相位差和离散，越大越小；</t>
+  </si>
+  <si>
+    <t>开启区域的斜率；gate diode导通的位置</t>
+  </si>
+  <si>
+    <t>S22幅值，越大越小；S21和S12相位差，越大越大；</t>
+  </si>
+  <si>
+    <t>Gate resistance (None Ohmic)</t>
+  </si>
+  <si>
+    <t>S11幅值，越大越小； S21和S12离散程度，越大越小；</t>
+  </si>
+  <si>
+    <t>S22和S12幅值，越大越小；</t>
+  </si>
+  <si>
+    <t>Drain inductance</t>
+  </si>
+  <si>
+    <t>Gate inductance</t>
+  </si>
+  <si>
+    <t>Source inductance</t>
+  </si>
+  <si>
+    <t>id-vg曲线的幅值</t>
+  </si>
+  <si>
+    <t>idvg开启电压的位置</t>
+  </si>
+  <si>
+    <t>扫描gate电压，idvd曲线的密集程度，为负时vg电压和i开启关系相反</t>
+  </si>
+  <si>
+    <t>idvd曲线集中在峰值gm处的vg电压</t>
+  </si>
+  <si>
+    <t>idvd曲线的密集程度</t>
+  </si>
+  <si>
+    <t>idvd幅值；idvg正向导通区域的幅值</t>
+  </si>
+  <si>
+    <t>有影响，但考虑到严谨性请勿tune</t>
+  </si>
+  <si>
+    <t>S11相位差，越大越大；S21和S12相位差，越大越大；</t>
+  </si>
+  <si>
+    <t>S22相位差，越大越小；S21幅值和相位差，越大越大；S12相位差，越大越大；</t>
+  </si>
+  <si>
+    <t>S11和S22相位差，越大越大；S21和S12在高频一侧曲线向内卷曲</t>
+  </si>
+  <si>
+    <t>idvd高电压处，未开启区域的电流扇开，非常微小</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,6 +654,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -525,11 +695,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,11 +1017,836 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B27D19-DD8A-884C-88AD-8DB5289C0FCC}">
+  <dimension ref="B2:BI39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="55.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="55.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="73" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="4" customWidth="1"/>
+    <col min="13" max="15" width="10.83203125" style="4"/>
+    <col min="16" max="16" width="10.83203125" style="5"/>
+    <col min="17" max="20" width="10.83203125" style="4"/>
+    <col min="21" max="21" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="10.83203125" style="4"/>
+    <col min="25" max="25" width="10.83203125" style="5"/>
+    <col min="26" max="33" width="10.83203125" style="4"/>
+    <col min="34" max="34" width="10.83203125" style="5"/>
+    <col min="35" max="42" width="10.83203125" style="4"/>
+    <col min="43" max="43" width="10.83203125" style="5"/>
+    <col min="44" max="51" width="10.83203125" style="4"/>
+    <col min="52" max="52" width="10.83203125" style="5"/>
+    <col min="53" max="60" width="10.83203125" style="4"/>
+    <col min="61" max="61" width="10.83203125" style="5"/>
+    <col min="62" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="Z8" s="7"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118C717B-6CE2-1C49-B11E-AF9547878177}">
   <dimension ref="A2:BJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>